<commit_message>
New cave ground material, sculpted rock shape and edges to look more natural
</commit_message>
<xml_diff>
--- a/oldgoldmine-scene/Tecniche.xlsx
+++ b/oldgoldmine-scene/Tecniche.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JackaL\source\repos\oldgoldmine-game\oldgoldmine-scene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331E9FF5-A1B0-49AB-AB55-AD13D0092ECE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975311DE-DCD7-440A-802A-B323E1CF20B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CA35FD49-B048-4DD9-AC47-1238A26E3A25}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="45">
   <si>
     <t>\</t>
   </si>
@@ -529,13 +529,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9734D29F-38DB-4CCD-84B1-0C16942DFD6A}">
   <dimension ref="A1:AK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="8" width="23.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.140625" customWidth="1"/>
@@ -544,7 +544,7 @@
     <col min="14" max="34" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1250,17 +1250,39 @@
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -2042,7 +2064,9 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>

</xml_diff>